<commit_message>
Final edits to exercise 1
</commit_message>
<xml_diff>
--- a/exercise1/solutions.xlsx
+++ b/exercise1/solutions.xlsx
@@ -1000,7 +1000,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1066,13 +1066,13 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1371,30 +1371,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1402,13 +1402,13 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>2.686E-5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>-1.8899999999999999E-6</v>
       </c>
       <c r="F3" s="1">
@@ -1422,13 +1422,13 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>2.3159999999999998E-5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>7.2399999999999998E-9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>-2.3099999999999999E-6</v>
       </c>
     </row>
@@ -1436,13 +1436,13 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>3.7419999999999997E-5</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>-2.3099999999999999E-6</v>
       </c>
     </row>
@@ -1450,13 +1450,13 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>4.2129999999999998E-5</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>9.0900000000000007E-9</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>-2.5299999999999999E-6</v>
       </c>
     </row>
@@ -1464,13 +1464,13 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1.365E-5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>2.9199999999999998E-9</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>-4.4999999999999998E-7</v>
       </c>
     </row>
@@ -1478,13 +1478,13 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>1.169E-5</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>3.2700000000000001E-9</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>2.7000000000000001E-7</v>
       </c>
     </row>
@@ -1492,13 +1492,13 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>1.6529999999999999E-5</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>3.7399999999999999E-9</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>3.3999999999999997E-7</v>
       </c>
     </row>
@@ -1506,13 +1506,13 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>2.8880000000000001E-5</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>7.6799999999999999E-9</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>2.3999999999999999E-6</v>
       </c>
     </row>
@@ -1520,13 +1520,13 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>4.507E-5</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>1.208E-8</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>-6.7499999999999997E-6</v>
       </c>
     </row>
@@ -1534,13 +1534,13 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>1.685E-5</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>5.2499999999999999E-9</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>-1.02E-6</v>
       </c>
     </row>
@@ -1548,13 +1548,13 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>2.6270000000000001E-5</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>9.46E-9</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>-3.1499999999999999E-6</v>
       </c>
     </row>
@@ -1562,39 +1562,39 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>3.3000000000000003E-5</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>0</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>67.430000000000007</v>
       </c>
       <c r="C19" s="1">
-        <f>B3+C3*($B$33-$F$3)+D3*($B$34-$G$3)</f>
+        <f t="shared" ref="C19:C30" si="0">B3+C3*($B$33-$F$3)+D3*($B$34-$G$3)</f>
         <v>2.3080189E-5</v>
       </c>
       <c r="D19" s="1">
@@ -1630,11 +1630,11 @@
         <v>0.16</v>
       </c>
       <c r="C20" s="1">
-        <f>B4+C4*($B$33-$F$3)+D4*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>1.4016316999999998E-5</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" ref="D20:D30" si="0">B20*C20</f>
+        <f t="shared" ref="D20:D30" si="1">B20*C20</f>
         <v>2.2426107199999998E-6</v>
       </c>
       <c r="E20">
@@ -1642,7 +1642,7 @@
         <v>80</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:F30" si="1">B20*E20</f>
+        <f t="shared" ref="F20:F30" si="2">B20*E20</f>
         <v>12.8</v>
       </c>
     </row>
@@ -1654,11 +1654,11 @@
         <v>6.86</v>
       </c>
       <c r="C21" s="1">
-        <f>B5+C5*($B$33-$F$3)+D5*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>3.2800230999999996E-5</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2500958465999999E-4</v>
       </c>
       <c r="E21">
@@ -1666,7 +1666,7 @@
         <v>102</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>699.72</v>
       </c>
     </row>
@@ -1678,11 +1678,11 @@
         <v>0.1</v>
       </c>
       <c r="C22" s="1">
-        <f>B6+C6*($B$33-$F$3)+D6*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>3.1390366499999995E-5</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1390366499999997E-6</v>
       </c>
       <c r="E22">
@@ -1690,7 +1690,7 @@
         <v>144</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.4</v>
       </c>
     </row>
@@ -1702,11 +1702,11 @@
         <v>0.54</v>
       </c>
       <c r="C23" s="1">
-        <f>B7+C7*($B$33-$F$3)+D7*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>1.0925483000000001E-5</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.8997608200000004E-6</v>
       </c>
       <c r="E23">
@@ -1714,7 +1714,7 @@
         <v>72</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38.880000000000003</v>
       </c>
     </row>
@@ -1726,11 +1726,11 @@
         <v>0.34</v>
       </c>
       <c r="C24" s="1">
-        <f>B8+C8*($B$33-$F$3)+D8*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>1.0186713500000001E-5</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.4634825900000005E-6</v>
       </c>
       <c r="E24">
@@ -1738,7 +1738,7 @@
         <v>140</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47.6</v>
       </c>
     </row>
@@ -1750,11 +1750,11 @@
         <v>2.29</v>
       </c>
       <c r="C25" s="1">
-        <f>B9+C9*($B$33-$F$3)+D9*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>1.4873027E-5</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.4059231830000001E-5</v>
       </c>
       <c r="E25">
@@ -1762,7 +1762,7 @@
         <v>56</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128.24</v>
       </c>
     </row>
@@ -1774,11 +1774,11 @@
         <v>2.29</v>
       </c>
       <c r="C26" s="1">
-        <f>B10+C10*($B$33-$F$3)+D10*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>2.8880912000000003E-5</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6137288480000014E-5</v>
       </c>
       <c r="E26">
@@ -1786,7 +1786,7 @@
         <v>62</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>141.97999999999999</v>
       </c>
     </row>
@@ -1798,11 +1798,11 @@
         <v>2.86</v>
       </c>
       <c r="C27" s="1">
-        <f>B11+C11*($B$33-$F$3)+D11*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>2.4022487000000004E-5</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8704312820000004E-5</v>
       </c>
       <c r="E27">
@@ -1810,7 +1810,7 @@
         <v>94</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>268.83999999999997</v>
       </c>
     </row>
@@ -1822,11 +1822,11 @@
         <v>0</v>
       </c>
       <c r="C28" s="1">
-        <f>B12+C12*($B$33-$F$3)+D12*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>1.15296395E-5</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E28">
@@ -1834,7 +1834,7 @@
         <v>30</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1846,11 +1846,11 @@
         <v>16.57</v>
       </c>
       <c r="C29" s="1">
-        <f>B13+C13*($B$33-$F$3)+D13*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>1.4059234000000002E-5</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3296150738000003E-4</v>
       </c>
       <c r="E29">
@@ -1858,7 +1858,7 @@
         <v>18</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>298.26</v>
       </c>
     </row>
@@ -1870,11 +1870,11 @@
         <v>0</v>
       </c>
       <c r="C30" s="1">
-        <f>B14+C14*($B$33-$F$3)+D14*($B$34-$G$3)</f>
+        <f t="shared" si="0"/>
         <v>3.3000000000000003E-5</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E30">
@@ -1882,19 +1882,19 @@
         <v>44</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="1">
         <f>SUM(D19:D30)</f>
         <v>2.19791396022E-3</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F31">
@@ -1926,7 +1926,7 @@
       <c r="B34">
         <v>2</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E34" s="1">
@@ -1935,7 +1935,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E35" s="1">
@@ -1944,28 +1944,28 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="6"/>
     </row>
     <row r="41" spans="1:6" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2001,11 +2001,11 @@
         <v>1.23</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" ref="C43:C53" si="2">B4+C4*($B$56-$F$3)+D4*($B$57-$G$3)</f>
+        <f t="shared" ref="C43:C53" si="3">B4+C4*($B$56-$F$3)+D4*($B$57-$G$3)</f>
         <v>1.6217277000000002E-5</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" ref="D43:D53" si="3">B43*C43</f>
+        <f t="shared" ref="D43:D53" si="4">B43*C43</f>
         <v>1.9947250710000002E-5</v>
       </c>
       <c r="E43">
@@ -2013,7 +2013,7 @@
         <v>80</v>
       </c>
       <c r="F43">
-        <f t="shared" ref="F43:F53" si="4">B43*E43</f>
+        <f t="shared" ref="F43:F53" si="5">B43*E43</f>
         <v>98.4</v>
       </c>
     </row>
@@ -2025,11 +2025,11 @@
         <v>10.49</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.2800230999999996E-5</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4407442318999996E-4</v>
       </c>
       <c r="E44">
@@ -2037,7 +2037,7 @@
         <v>102</v>
       </c>
       <c r="F44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1069.98</v>
       </c>
     </row>
@@ -2049,11 +2049,11 @@
         <v>0.1</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.4153726499999994E-5</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4153726499999996E-6</v>
       </c>
       <c r="E45">
@@ -2061,7 +2061,7 @@
         <v>144</v>
       </c>
       <c r="F45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.4</v>
       </c>
     </row>
@@ -2073,11 +2073,11 @@
         <v>0.54</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1813162999999999E-5</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.3791080200000003E-6</v>
       </c>
       <c r="E46">
@@ -2085,7 +2085,7 @@
         <v>72</v>
       </c>
       <c r="F46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>38.880000000000003</v>
       </c>
     </row>
@@ -2097,11 +2097,11 @@
         <v>6.79</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.11807935E-5</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.5917587865000004E-5</v>
       </c>
       <c r="E47">
@@ -2109,7 +2109,7 @@
         <v>140</v>
       </c>
       <c r="F47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>950.6</v>
       </c>
     </row>
@@ -2121,11 +2121,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6009987000000002E-5</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.522197140000001E-5</v>
       </c>
       <c r="E48">
@@ -2133,7 +2133,7 @@
         <v>56</v>
       </c>
       <c r="F48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>123.20000000000002</v>
       </c>
     </row>
@@ -2145,11 +2145,11 @@
         <v>2.29</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1215632000000001E-5</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.1483797280000002E-5</v>
       </c>
       <c r="E49">
@@ -2157,7 +2157,7 @@
         <v>62</v>
       </c>
       <c r="F49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>141.97999999999999</v>
       </c>
     </row>
@@ -2169,11 +2169,11 @@
         <v>2.86</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7694807E-5</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.920714802E-5</v>
       </c>
       <c r="E50">
@@ -2181,7 +2181,7 @@
         <v>94</v>
       </c>
       <c r="F50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>268.83999999999997</v>
       </c>
     </row>
@@ -2193,11 +2193,11 @@
         <v>0</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.31256395E-5</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E51">
@@ -2205,7 +2205,7 @@
         <v>30</v>
       </c>
       <c r="F51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2217,11 +2217,11 @@
         <v>20</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6935074000000002E-5</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3870148000000004E-4</v>
       </c>
       <c r="E52">
@@ -2229,7 +2229,7 @@
         <v>18</v>
       </c>
       <c r="F52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>360</v>
       </c>
     </row>
@@ -2241,11 +2241,11 @@
         <v>0</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3000000000000003E-5</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E53">
@@ -2253,19 +2253,19 @@
         <v>44</v>
       </c>
       <c r="F53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D54" s="1">
         <f>SUM(D42:D53)</f>
         <v>2.209138250635E-3</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F54">
@@ -2297,7 +2297,7 @@
       <c r="B57">
         <v>2</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E57" s="1">
@@ -2306,7 +2306,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E58" s="1">
@@ -2315,22 +2315,22 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2360,7 +2360,7 @@
         <v>3350</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D68" si="5">B66*C66</f>
+        <f t="shared" ref="D66:D68" si="6">B66*C66</f>
         <v>67</v>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
         <v>2620</v>
       </c>
       <c r="D67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>786</v>
       </c>
     </row>
@@ -2392,12 +2392,12 @@
         <v>2591.7848028181265</v>
       </c>
       <c r="D68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1580.9887297190571</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D69">
@@ -2421,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2435,16 +2435,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B3">
@@ -2452,13 +2452,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B5">
         <v>159.6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E5">
@@ -2466,13 +2466,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B6">
         <v>-173.3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E6">
@@ -2480,13 +2480,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B7">
         <v>72.099999999999994</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E7">
@@ -2494,13 +2494,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B8">
         <v>75.7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E8">
@@ -2508,13 +2508,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B9">
         <v>-39.9</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E9">
@@ -2522,13 +2522,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B10">
         <v>-84.1</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>63</v>
       </c>
       <c r="E10">
@@ -2536,7 +2536,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B11">
@@ -2544,13 +2544,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B13">
         <v>-2.4300000000000002</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E13">
@@ -2558,7 +2558,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B14">
@@ -2566,7 +2566,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B15">
@@ -2574,31 +2574,31 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="J18" s="3" t="s">
+      <c r="G18" s="2"/>
+      <c r="J18" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E19">
@@ -2609,7 +2609,7 @@
         <f>B5*E19</f>
         <v>8734.9079999999994</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I19">
@@ -2620,16 +2620,16 @@
         <f>E5*I19</f>
         <v>147.125</v>
       </c>
-      <c r="K19" s="3"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B20">
         <v>53.5</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E20">
@@ -2640,7 +2640,7 @@
         <f t="shared" ref="F20:F25" si="0">B6*E20</f>
         <v>-1817.9170000000001</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I20">
@@ -2653,43 +2653,43 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B21">
         <v>1.23</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E21">
         <f>B23+B24+B25</f>
-        <v>0.76</v>
+        <v>1.76</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>54.795999999999999</v>
-      </c>
-      <c r="H21" s="3" t="s">
+        <v>126.89599999999999</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>75</v>
       </c>
       <c r="I21">
         <f>B23+B24+B26</f>
-        <v>7.48</v>
+        <v>8.48</v>
       </c>
       <c r="J21">
         <f t="shared" si="1"/>
-        <v>62.08400000000001</v>
+        <v>70.384000000000015</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B22">
         <v>10.49</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E22">
@@ -2700,7 +2700,7 @@
         <f t="shared" si="0"/>
         <v>514.00300000000004</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>76</v>
       </c>
       <c r="I22">
@@ -2713,13 +2713,13 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B23">
-        <v>0.54</v>
-      </c>
-      <c r="D23" s="3" t="s">
+        <v>1.54</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E23">
@@ -2730,7 +2730,7 @@
         <f t="shared" si="0"/>
         <v>-87.78</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>77</v>
       </c>
       <c r="I23">
@@ -2743,143 +2743,143 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B24">
         <v>0.15</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E24">
         <f>B28+B29+B30</f>
-        <v>15.879999999999999</v>
+        <v>22.29</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>-1335.5079999999998</v>
-      </c>
-      <c r="H24" s="3" t="s">
+        <v>-1874.5889999999997</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>78</v>
       </c>
       <c r="I24">
         <f>LN(1+B29+B30)</f>
-        <v>2.6803363625346943</v>
+        <v>3.044522437723423</v>
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
-        <v>-265.6213335271882</v>
+        <v>-301.71217357839123</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B25">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E25">
         <f>B29+B30+LN(1+B29)</f>
-        <v>16.270336362534692</v>
+        <v>23.044522437723423</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>2302.2525952986589</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3" t="s">
+        <v>3260.7999249378645</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J25">
         <f>SUM(J19:J24)</f>
-        <v>86.686666472811794</v>
+        <v>58.895826421608774</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B26">
         <v>6.79</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F26">
         <f>SUM(F19:F25)</f>
-        <v>8364.7545952986584</v>
+        <v>8856.3209249378633</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B28">
         <v>2.29</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E28">
         <f>E19*I21</f>
-        <v>409.38040000000001</v>
+        <v>464.11039999999997</v>
       </c>
       <c r="F28">
         <f>E28*B13</f>
-        <v>-994.79437200000007</v>
-      </c>
-      <c r="H28" s="3" t="s">
+        <v>-1127.788272</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>82</v>
       </c>
       <c r="I28">
         <f>(E20+I21+I22-B25)*(I23+B29+B30)</f>
-        <v>376.67399999999998</v>
+        <v>530.66499999999996</v>
       </c>
       <c r="J28">
         <f>E13*I28</f>
-        <v>113.00219999999999</v>
+        <v>159.19949999999997</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B29">
-        <v>13.59</v>
-      </c>
-      <c r="D29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E29">
         <f>(I19+I20+B25)*(I23+B29)</f>
-        <v>1223.5346</v>
+        <v>1642.0434999999998</v>
       </c>
       <c r="F29">
         <f>E29*B14</f>
-        <v>-1113.4164860000001</v>
+        <v>-1494.2595849999998</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E30">
@@ -2892,208 +2892,208 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B31">
         <v>2.86</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F31">
         <f>SUM(F28:F30)</f>
-        <v>-1157.3972580000002</v>
+        <v>-1671.2342569999994</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B33">
         <v>1352.15</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F33">
         <f>F26+F31</f>
-        <v>7207.3573372986584</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3" t="s">
+        <v>7185.0866679378641</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2" t="s">
         <v>87</v>
       </c>
       <c r="J33">
         <f>J25+J28</f>
-        <v>199.68886647281178</v>
-      </c>
-      <c r="L33" s="3" t="s">
+        <v>218.09532642160875</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>86</v>
       </c>
       <c r="M33">
         <f>10^(B3+F33/(B33-J33))</f>
-        <v>50.568865867157555</v>
+        <v>61.059015423788821</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="37" spans="1:13" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G37" s="3"/>
-      <c r="J37" s="3" t="s">
+      <c r="G37" s="2"/>
+      <c r="J37" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E38">
         <f>B39+B40</f>
-        <v>54.73</v>
+        <v>67.59</v>
       </c>
       <c r="F38">
-        <f>B5*E38</f>
-        <v>8734.9079999999994</v>
-      </c>
-      <c r="H38" s="3" t="s">
+        <f t="shared" ref="F38:F44" si="2">B5*E38</f>
+        <v>10787.364</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I38">
         <f>B39</f>
-        <v>53.5</v>
+        <v>67.430000000000007</v>
       </c>
       <c r="J38">
-        <f>E5*I38</f>
-        <v>147.125</v>
-      </c>
-      <c r="K38" s="3"/>
+        <f t="shared" ref="J38:J43" si="3">E5*I38</f>
+        <v>185.4325</v>
+      </c>
+      <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B39">
-        <v>53.5</v>
-      </c>
-      <c r="D39" s="3" t="s">
+        <v>67.430000000000007</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E39">
         <f>B41</f>
-        <v>10.49</v>
+        <v>6.86</v>
       </c>
       <c r="F39">
-        <f>B6*E39</f>
-        <v>-1817.9170000000001</v>
-      </c>
-      <c r="H39" s="3" t="s">
+        <f t="shared" si="2"/>
+        <v>-1188.8380000000002</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I39">
         <f>B40+B41</f>
-        <v>11.72</v>
+        <v>7.0200000000000005</v>
       </c>
       <c r="J39">
-        <f>E6*I39</f>
-        <v>184.00399999999999</v>
+        <f t="shared" si="3"/>
+        <v>110.214</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B40">
-        <v>1.23</v>
-      </c>
-      <c r="D40" s="3" t="s">
+        <v>0.16</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E40">
         <f>B42+B43+B44</f>
-        <v>0.76</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="F40">
-        <f>B7*E40</f>
-        <v>54.795999999999999</v>
-      </c>
-      <c r="H40" s="3" t="s">
+        <f t="shared" si="2"/>
+        <v>33.887</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>75</v>
       </c>
       <c r="I40">
         <f>B42+B43+B45</f>
-        <v>7.48</v>
+        <v>0.74</v>
       </c>
       <c r="J40">
-        <f>E7*I40</f>
-        <v>62.08400000000001</v>
+        <f t="shared" si="3"/>
+        <v>6.1420000000000003</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B41">
-        <v>10.49</v>
-      </c>
-      <c r="D41" s="3" t="s">
+        <v>6.86</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E41">
         <f>B45</f>
-        <v>6.79</v>
+        <v>0.34</v>
       </c>
       <c r="F41">
-        <f>B8*E41</f>
-        <v>514.00300000000004</v>
-      </c>
-      <c r="H41" s="3" t="s">
+        <f t="shared" si="2"/>
+        <v>25.738000000000003</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>76</v>
       </c>
       <c r="I41">
         <f>B46</f>
-        <v>2.2000000000000002</v>
+        <v>2.29</v>
       </c>
       <c r="J41">
-        <f>E8*I41</f>
-        <v>22.44</v>
+        <f t="shared" si="3"/>
+        <v>23.357999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B42">
-        <v>0.54</v>
-      </c>
-      <c r="D42" s="3" t="s">
+        <v>0.25</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E42">
         <f>B46</f>
-        <v>2.2000000000000002</v>
+        <v>2.29</v>
       </c>
       <c r="F42">
-        <f>B9*E42</f>
-        <v>-87.78</v>
-      </c>
-      <c r="H42" s="3" t="s">
+        <f t="shared" si="2"/>
+        <v>-91.370999999999995</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>77</v>
       </c>
       <c r="I42">
@@ -3101,218 +3101,218 @@
         <v>5.15</v>
       </c>
       <c r="J42">
-        <f>E9*I42</f>
+        <f t="shared" si="3"/>
         <v>-63.345000000000006</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B43">
         <v>0.15</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E43">
         <f>B47+B48+B49</f>
-        <v>15.879999999999999</v>
+        <v>18.86</v>
       </c>
       <c r="F43">
-        <f>B10*E43</f>
-        <v>-1335.5079999999998</v>
-      </c>
-      <c r="H43" s="3" t="s">
+        <f t="shared" si="2"/>
+        <v>-1586.1259999999997</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>78</v>
       </c>
       <c r="I43">
         <f>LN(1+B48+B49)</f>
-        <v>2.6803363625346943</v>
+        <v>2.866192902199006</v>
       </c>
       <c r="J43">
-        <f>E10*I43</f>
-        <v>-265.6213335271882</v>
+        <f t="shared" si="3"/>
+        <v>-284.03971660792149</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B44">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E44">
         <f>B48+B49+LN(1+B48)</f>
-        <v>16.270336362534692</v>
+        <v>19.436192902199007</v>
       </c>
       <c r="F44">
-        <f>B11*E44</f>
-        <v>2302.2525952986589</v>
-      </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3" t="s">
+        <f t="shared" si="2"/>
+        <v>2750.2212956611597</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J44">
         <f>SUM(J38:J43)</f>
-        <v>86.686666472811794</v>
+        <v>-22.238216607921515</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B45">
-        <v>6.79</v>
-      </c>
-      <c r="E45" s="3" t="s">
+        <v>0.34</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F45">
         <f>SUM(F38:F44)</f>
-        <v>8364.7545952986584</v>
+        <v>10730.875295661161</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B46">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D46" s="3"/>
+        <v>2.29</v>
+      </c>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B47">
         <v>2.29</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E47">
         <f>E38*I40</f>
-        <v>409.38040000000001</v>
+        <v>50.016600000000004</v>
       </c>
       <c r="F47">
         <f>E47*B13</f>
-        <v>-994.79437200000007</v>
-      </c>
-      <c r="H47" s="3" t="s">
+        <v>-121.54033800000002</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>82</v>
       </c>
       <c r="I47">
         <f>(E39+I40+I41-B44)*(I42+B48+B49)</f>
-        <v>376.67399999999998</v>
+        <v>213.29040000000001</v>
       </c>
       <c r="J47">
         <f>E13*I47</f>
-        <v>113.00219999999999</v>
+        <v>63.987119999999997</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B48">
-        <v>13.59</v>
-      </c>
-      <c r="D48" s="3" t="s">
+        <v>16.57</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E48">
         <f>(I38+I39+B44)*(I42+B48)</f>
-        <v>1223.5346</v>
+        <v>1618.5743999999997</v>
       </c>
       <c r="F48">
         <f>E48*B14</f>
-        <v>-1113.4164860000001</v>
+        <v>-1472.9027039999999</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E49">
         <f>E39*I42</f>
-        <v>54.023500000000006</v>
+        <v>35.329000000000001</v>
       </c>
       <c r="F49">
         <f>E49*B15</f>
-        <v>950.81360000000018</v>
+        <v>621.79040000000009</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B50">
         <v>2.86</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F50">
         <f>SUM(F47:F49)</f>
-        <v>-1157.3972580000002</v>
+        <v>-972.65264199999979</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B52">
         <v>1048.95</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F52">
         <f>F45+F50</f>
-        <v>7207.3573372986584</v>
-      </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3" t="s">
+        <v>9758.2226536611615</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2" t="s">
         <v>87</v>
       </c>
       <c r="J52">
         <f>J44+J47</f>
-        <v>199.68886647281178</v>
-      </c>
-      <c r="L52" s="3" t="s">
+        <v>41.748903392078482</v>
+      </c>
+      <c r="L52" s="2" t="s">
         <v>86</v>
       </c>
       <c r="M52">
         <f>10^(B3+F52/(B52-J52))</f>
-        <v>8642.1333079018168</v>
+        <v>137548.27622847148</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3341,29 +3341,29 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B60">
         <f>SUM(B57:B59)</f>
         <v>0.39</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>86</v>
       </c>
       <c r="E60">
         <f>M52*(1-B60/0.4)^(-2.5*0.4)</f>
-        <v>345685.33231607237</v>
+        <v>5501931.0491388543</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B65">

</xml_diff>